<commit_message>
Mensagem explicando as mudanças
</commit_message>
<xml_diff>
--- a/Dados_Comerciais.xlsx
+++ b/Dados_Comerciais.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Drive\Área de Trabalho\Projeto_Series_Temporais\Projeto_Series_Temporais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA490698-EE98-42B9-9F0E-8E0B90C97FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC12FBCF-2C8C-4BC1-A58E-607F96EB2CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="1" r:id="rId1"/>
     <sheet name="Exercicios" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Vendas!$E$1:$E$458</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Vendas!$A$1:$N$458</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -1733,7 +1733,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1828,7 +1828,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1837,9 +1837,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -2131,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N458"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="122" zoomScaleNormal="122" zoomScalePageLayoutView="122" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="122" zoomScaleNormal="122" zoomScalePageLayoutView="122" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,7 +2272,7 @@
         <v>1006</v>
       </c>
       <c r="K3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" s="3">
         <v>40909</v>
@@ -2362,7 +2361,7 @@
         <v>1003</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="3">
         <v>40971</v>
@@ -2406,7 +2405,7 @@
         <v>1004</v>
       </c>
       <c r="K6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L6" s="3">
         <v>41003</v>
@@ -2450,7 +2449,7 @@
         <v>1005</v>
       </c>
       <c r="K7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L7" s="3">
         <v>41033</v>
@@ -2494,7 +2493,7 @@
         <v>1006</v>
       </c>
       <c r="K8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L8" s="3">
         <v>41064</v>
@@ -2582,7 +2581,7 @@
         <v>1003</v>
       </c>
       <c r="K10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L10" s="3">
         <v>41125</v>
@@ -2626,7 +2625,7 @@
         <v>1002</v>
       </c>
       <c r="K11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L11" s="3">
         <v>41156</v>
@@ -2670,7 +2669,7 @@
         <v>1009</v>
       </c>
       <c r="K12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L12" s="3">
         <v>41156</v>
@@ -2714,7 +2713,7 @@
         <v>1006</v>
       </c>
       <c r="K13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L13" s="3">
         <v>41217</v>
@@ -2758,7 +2757,7 @@
         <v>1006</v>
       </c>
       <c r="K14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L14" s="3">
         <v>41217</v>
@@ -2802,7 +2801,7 @@
         <v>1003</v>
       </c>
       <c r="K15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L15" s="3">
         <v>41247</v>
@@ -2890,7 +2889,7 @@
         <v>1005</v>
       </c>
       <c r="K17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L17" s="3">
         <v>41276</v>
@@ -2934,7 +2933,7 @@
         <v>1006</v>
       </c>
       <c r="K18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L18" s="3">
         <v>41307</v>
@@ -2978,7 +2977,7 @@
         <v>1007</v>
       </c>
       <c r="K19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L19" s="3">
         <v>41335</v>
@@ -3022,7 +3021,7 @@
         <v>1003</v>
       </c>
       <c r="K20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L20" s="3">
         <v>41366</v>
@@ -3066,7 +3065,7 @@
         <v>1002</v>
       </c>
       <c r="K21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L21" s="3">
         <v>41396</v>
@@ -3110,7 +3109,7 @@
         <v>1009</v>
       </c>
       <c r="K22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L22" s="3">
         <v>41427</v>
@@ -3154,7 +3153,7 @@
         <v>1006</v>
       </c>
       <c r="K23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L23" s="3">
         <v>41457</v>
@@ -3198,7 +3197,7 @@
         <v>1006</v>
       </c>
       <c r="K24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L24" s="3">
         <v>41488</v>
@@ -3242,7 +3241,7 @@
         <v>1003</v>
       </c>
       <c r="K25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L25" s="3">
         <v>41519</v>
@@ -3330,7 +3329,7 @@
         <v>1005</v>
       </c>
       <c r="K27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L27" s="3">
         <v>41580</v>
@@ -3374,7 +3373,7 @@
         <v>1006</v>
       </c>
       <c r="K28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L28" s="3">
         <v>41610</v>
@@ -3418,7 +3417,7 @@
         <v>1007</v>
       </c>
       <c r="K29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L29" s="3">
         <v>41276</v>
@@ -3462,7 +3461,7 @@
         <v>1003</v>
       </c>
       <c r="K30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L30" s="3">
         <v>41307</v>
@@ -3506,7 +3505,7 @@
         <v>1002</v>
       </c>
       <c r="K31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L31" s="3">
         <v>41335</v>
@@ -3550,7 +3549,7 @@
         <v>1001</v>
       </c>
       <c r="K32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L32" s="3">
         <v>41366</v>
@@ -3594,7 +3593,7 @@
         <v>1001</v>
       </c>
       <c r="K33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L33" s="3">
         <v>41396</v>
@@ -3770,7 +3769,7 @@
         <v>1004</v>
       </c>
       <c r="K37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L37" s="3">
         <v>41519</v>
@@ -3814,7 +3813,7 @@
         <v>1005</v>
       </c>
       <c r="K38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L38" s="3">
         <v>41549</v>
@@ -3858,7 +3857,7 @@
         <v>1006</v>
       </c>
       <c r="K39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L39" s="3">
         <v>41580</v>
@@ -3946,7 +3945,7 @@
         <v>1008</v>
       </c>
       <c r="K41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L41" s="3">
         <v>40909</v>
@@ -22307,7 +22306,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E458" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:N458" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -22317,7 +22316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ACC56D-F1B4-4802-80C3-DB77F39C0530}">
   <dimension ref="A1:Q459"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
+    <sheetView topLeftCell="G11" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -22381,13 +22380,13 @@
       <c r="J2" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="6" t="s">
         <v>551</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>551</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -22396,7 +22395,7 @@
       <c r="P2" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="6" t="s">
         <v>551</v>
       </c>
     </row>
@@ -23018,25 +23017,25 @@
         <f>VLOOKUP(F15,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <v>0</v>
       </c>
       <c r="K15">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>1</v>
-      </c>
-      <c r="L15" s="11">
+        <v>5</v>
+      </c>
+      <c r="L15" s="10">
         <f>M15*60*60*24</f>
         <v>240.00000000000006</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="10">
         <f ca="1">L15/K15</f>
-        <v>240.00000000000006</v>
-      </c>
-      <c r="O15" s="11">
+        <v>48.000000000000014</v>
+      </c>
+      <c r="O15" s="10">
         <f ca="1">SUMPRODUCT(K15,L15)/SUM(K15)</f>
         <v>240.00000000000006</v>
       </c>
@@ -23068,25 +23067,25 @@
         <f>VLOOKUP(F16,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="8">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="K16">
         <f t="shared" ref="K16:K62" ca="1" si="0">RANDBETWEEN(1,5)</f>
         <v>1</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <f t="shared" ref="L16:L62" si="1">M16*60*60*24</f>
         <v>420</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="10">
         <f t="shared" ref="N16:N62" ca="1" si="2">L16/K16</f>
         <v>420</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="10">
         <f t="shared" ref="O16:O62" ca="1" si="3">SUMPRODUCT(K16,L16)/SUM(K16)</f>
         <v>420</v>
       </c>
@@ -23118,25 +23117,25 @@
         <f>VLOOKUP(F17,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L17" s="11">
+        <v>5</v>
+      </c>
+      <c r="L17" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>87.999999999999986</v>
-      </c>
-      <c r="O17" s="11">
+        <v>35.199999999999996</v>
+      </c>
+      <c r="O17" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -23168,27 +23167,27 @@
         <f>VLOOKUP(F18,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <v>6.25E-2</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L18" s="11">
+        <v>5</v>
+      </c>
+      <c r="L18" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>80.000000000000014</v>
-      </c>
-      <c r="O18" s="11">
+        <v>48.000000000000014</v>
+      </c>
+      <c r="O18" s="10">
         <f t="shared" ca="1" si="3"/>
-        <v>240.00000000000009</v>
+        <v>240.00000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -23218,25 +23217,25 @@
         <f>VLOOKUP(F19,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L19" s="11">
+        <v>3</v>
+      </c>
+      <c r="L19" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>420</v>
-      </c>
-      <c r="O19" s="11">
+        <v>140</v>
+      </c>
+      <c r="O19" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -23268,25 +23267,25 @@
         <f>VLOOKUP(F20,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <v>0.104166666666667</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L20" s="11">
+        <v>3</v>
+      </c>
+      <c r="L20" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43.999999999999993</v>
-      </c>
-      <c r="O20" s="11">
+        <v>58.666666666666657</v>
+      </c>
+      <c r="O20" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -23318,25 +23317,25 @@
         <f>VLOOKUP(F21,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="8">
         <v>0.125</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L21" s="11">
+        <v>4</v>
+      </c>
+      <c r="L21" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>240.00000000000006</v>
-      </c>
-      <c r="O21" s="11">
+        <v>60.000000000000014</v>
+      </c>
+      <c r="O21" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -23368,25 +23367,25 @@
         <f>VLOOKUP(F22,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="8">
         <v>0.14583333333333301</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L22" s="11">
+        <v>2</v>
+      </c>
+      <c r="L22" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
-      </c>
-      <c r="O22" s="11">
+        <v>210</v>
+      </c>
+      <c r="O22" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -23418,25 +23417,25 @@
         <f>VLOOKUP(F23,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="8">
         <v>0.16666666666666699</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L23" s="11">
+        <v>5</v>
+      </c>
+      <c r="L23" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>87.999999999999986</v>
-      </c>
-      <c r="O23" s="11">
+        <v>35.199999999999996</v>
+      </c>
+      <c r="O23" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -23468,27 +23467,27 @@
         <f>VLOOKUP(F24,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <v>0.1875</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L24" s="11">
+        <v>1</v>
+      </c>
+      <c r="L24" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>80.000000000000014</v>
-      </c>
-      <c r="O24" s="11">
+        <v>240.00000000000006</v>
+      </c>
+      <c r="O24" s="10">
         <f t="shared" ca="1" si="3"/>
-        <v>240.00000000000009</v>
+        <v>240.00000000000006</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -23518,25 +23517,25 @@
         <f>VLOOKUP(F25,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="8">
         <v>0.20833333333333301</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N25" s="11">
+      <c r="N25" s="10">
         <f t="shared" ca="1" si="2"/>
         <v>140</v>
       </c>
-      <c r="O25" s="11">
+      <c r="O25" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -23568,25 +23567,25 @@
         <f>VLOOKUP(F26,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="8">
         <v>0.22916666666666699</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L26" s="11">
+        <v>5</v>
+      </c>
+      <c r="L26" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>58.666666666666657</v>
-      </c>
-      <c r="O26" s="11">
+        <v>35.199999999999996</v>
+      </c>
+      <c r="O26" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -23618,27 +23617,27 @@
         <f>VLOOKUP(F27,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="8">
         <v>0.25</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L27" s="11">
+        <v>3</v>
+      </c>
+      <c r="L27" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>48.000000000000014</v>
-      </c>
-      <c r="O27" s="11">
+        <v>80.000000000000014</v>
+      </c>
+      <c r="O27" s="10">
         <f t="shared" ca="1" si="3"/>
-        <v>240.00000000000006</v>
+        <v>240.00000000000009</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -23668,25 +23667,25 @@
         <f>VLOOKUP(F28,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="8">
         <v>0.27083333333333298</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L28" s="11">
+        <v>3</v>
+      </c>
+      <c r="L28" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N28" s="11">
+      <c r="N28" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="O28" s="11">
+        <v>140</v>
+      </c>
+      <c r="O28" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -23718,25 +23717,25 @@
         <f>VLOOKUP(F29,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="8">
         <v>0.29166666666666702</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L29" s="11">
+        <v>3</v>
+      </c>
+      <c r="L29" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>87.999999999999986</v>
-      </c>
-      <c r="O29" s="11">
+        <v>58.666666666666657</v>
+      </c>
+      <c r="O29" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -23768,25 +23767,25 @@
         <f>VLOOKUP(F30,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="8">
         <v>0.3125</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L30" s="11">
+        <v>4</v>
+      </c>
+      <c r="L30" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N30" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>240.00000000000006</v>
-      </c>
-      <c r="O30" s="11">
+        <v>60.000000000000014</v>
+      </c>
+      <c r="O30" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -23818,25 +23817,25 @@
         <f>VLOOKUP(F31,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="8">
         <v>0.33333333333333298</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L31" s="11">
+        <v>1</v>
+      </c>
+      <c r="L31" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N31" s="11">
+      <c r="N31" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="O31" s="11">
+        <v>420</v>
+      </c>
+      <c r="O31" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -23868,25 +23867,25 @@
         <f>VLOOKUP(F32,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="8">
         <v>0.35416666666666702</v>
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L32" s="11">
+        <v>4</v>
+      </c>
+      <c r="L32" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N32" s="11">
+      <c r="N32" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>35.199999999999996</v>
-      </c>
-      <c r="O32" s="11">
+        <v>43.999999999999993</v>
+      </c>
+      <c r="O32" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -23918,25 +23917,25 @@
         <f>VLOOKUP(F33,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33" s="8">
         <v>0.375</v>
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L33" s="11">
+        <v>1</v>
+      </c>
+      <c r="L33" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N33" s="11">
+      <c r="N33" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>120.00000000000003</v>
-      </c>
-      <c r="O33" s="11">
+        <v>240.00000000000006</v>
+      </c>
+      <c r="O33" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -23968,25 +23967,25 @@
         <f>VLOOKUP(F34,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J34" s="9">
+      <c r="J34" s="8">
         <v>0.39583333333333298</v>
       </c>
       <c r="K34">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L34" s="11">
+        <v>3</v>
+      </c>
+      <c r="L34" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N34" s="11">
+      <c r="N34" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="O34" s="11">
+        <v>140</v>
+      </c>
+      <c r="O34" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -24018,25 +24017,25 @@
         <f>VLOOKUP(F35,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="8">
         <v>0.41666666666666702</v>
       </c>
       <c r="K35">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L35" s="11">
+        <v>1</v>
+      </c>
+      <c r="L35" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M35" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N35" s="11">
+      <c r="N35" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>58.666666666666657</v>
-      </c>
-      <c r="O35" s="11">
+        <v>175.99999999999997</v>
+      </c>
+      <c r="O35" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -24068,25 +24067,25 @@
         <f>VLOOKUP(F36,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J36" s="9">
+      <c r="J36" s="8">
         <v>0.4375</v>
       </c>
       <c r="K36">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="L36" s="11">
+      <c r="L36" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M36" s="10">
+      <c r="M36" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N36" s="11">
+      <c r="N36" s="10">
         <f t="shared" ca="1" si="2"/>
         <v>48.000000000000014</v>
       </c>
-      <c r="O36" s="11">
+      <c r="O36" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -24118,25 +24117,25 @@
         <f>VLOOKUP(F37,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J37" s="9">
+      <c r="J37" s="8">
         <v>0.45833333333333298</v>
       </c>
       <c r="K37">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L37" s="11">
+        <v>3</v>
+      </c>
+      <c r="L37" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N37" s="11">
+      <c r="N37" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="O37" s="11">
+        <v>140</v>
+      </c>
+      <c r="O37" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -24168,25 +24167,25 @@
         <f>VLOOKUP(F38,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38" s="8">
         <v>0.47916666666666702</v>
       </c>
       <c r="K38">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L38" s="11">
+        <v>2</v>
+      </c>
+      <c r="L38" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N38" s="11">
+      <c r="N38" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>35.199999999999996</v>
-      </c>
-      <c r="O38" s="11">
+        <v>87.999999999999986</v>
+      </c>
+      <c r="O38" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -24218,25 +24217,25 @@
         <f>VLOOKUP(F39,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39" s="8">
         <v>0.5</v>
       </c>
       <c r="K39">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L39" s="11">
+        <v>5</v>
+      </c>
+      <c r="L39" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N39" s="11">
+      <c r="N39" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>60.000000000000014</v>
-      </c>
-      <c r="O39" s="11">
+        <v>48.000000000000014</v>
+      </c>
+      <c r="O39" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -24268,25 +24267,25 @@
         <f>VLOOKUP(F40,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J40" s="9">
+      <c r="J40" s="8">
         <v>0.52083333333333304</v>
       </c>
       <c r="K40">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L40" s="11">
+        <v>5</v>
+      </c>
+      <c r="L40" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M40" s="10">
+      <c r="M40" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N40" s="11">
+      <c r="N40" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="O40" s="11">
+        <v>84</v>
+      </c>
+      <c r="O40" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -24318,25 +24317,25 @@
         <f>VLOOKUP(F41,Vendas!A:C,3,0)</f>
         <v>Eletrodomésticos</v>
       </c>
-      <c r="J41" s="9">
+      <c r="J41" s="8">
         <v>0.54166666666666696</v>
       </c>
       <c r="K41">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="L41" s="11">
+      <c r="L41" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M41" s="10">
+      <c r="M41" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N41" s="11">
+      <c r="N41" s="10">
         <f t="shared" ca="1" si="2"/>
         <v>87.999999999999986</v>
       </c>
-      <c r="O41" s="11">
+      <c r="O41" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -24368,25 +24367,25 @@
         <f>VLOOKUP(F42,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J42" s="9">
+      <c r="J42" s="8">
         <v>0.5625</v>
       </c>
       <c r="K42">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="L42" s="11">
+      <c r="L42" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M42" s="10">
+      <c r="M42" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N42" s="11">
+      <c r="N42" s="10">
         <f t="shared" ca="1" si="2"/>
         <v>48.000000000000014</v>
       </c>
-      <c r="O42" s="11">
+      <c r="O42" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -24418,25 +24417,25 @@
         <f>VLOOKUP(F43,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J43" s="9">
+      <c r="J43" s="8">
         <v>0.58333333333333304</v>
       </c>
       <c r="K43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L43" s="11">
+        <v>1</v>
+      </c>
+      <c r="L43" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M43" s="10">
+      <c r="M43" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N43" s="11">
+      <c r="N43" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>210</v>
-      </c>
-      <c r="O43" s="11">
+        <v>420</v>
+      </c>
+      <c r="O43" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -24468,25 +24467,25 @@
         <f>VLOOKUP(F44,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J44" s="9">
+      <c r="J44" s="8">
         <v>0.60416666666666696</v>
       </c>
       <c r="K44">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L44" s="11">
+        <v>2</v>
+      </c>
+      <c r="L44" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M44" s="10">
+      <c r="M44" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N44" s="11">
+      <c r="N44" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43.999999999999993</v>
-      </c>
-      <c r="O44" s="11">
+        <v>87.999999999999986</v>
+      </c>
+      <c r="O44" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -24518,25 +24517,25 @@
         <f>VLOOKUP(F45,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J45" s="9">
+      <c r="J45" s="8">
         <v>0.625</v>
       </c>
       <c r="K45">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L45" s="11">
+        <v>5</v>
+      </c>
+      <c r="L45" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M45" s="10">
+      <c r="M45" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N45" s="11">
+      <c r="N45" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>240.00000000000006</v>
-      </c>
-      <c r="O45" s="11">
+        <v>48.000000000000014</v>
+      </c>
+      <c r="O45" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -24568,25 +24567,25 @@
         <f>VLOOKUP(F46,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J46" s="9">
+      <c r="J46" s="8">
         <v>0.64583333333333304</v>
       </c>
       <c r="K46">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L46" s="11">
+        <v>3</v>
+      </c>
+      <c r="L46" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M46" s="10">
+      <c r="M46" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N46" s="11">
+      <c r="N46" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="O46" s="11">
+        <v>140</v>
+      </c>
+      <c r="O46" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -24618,25 +24617,25 @@
         <f>VLOOKUP(F47,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J47" s="9">
+      <c r="J47" s="8">
         <v>0.66666666666666696</v>
       </c>
       <c r="K47">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L47" s="11">
+        <v>1</v>
+      </c>
+      <c r="L47" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M47" s="10">
+      <c r="M47" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N47" s="11">
+      <c r="N47" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>35.199999999999996</v>
-      </c>
-      <c r="O47" s="11">
+        <v>175.99999999999997</v>
+      </c>
+      <c r="O47" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -24668,25 +24667,25 @@
         <f>VLOOKUP(F48,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J48" s="9">
+      <c r="J48" s="8">
         <v>0.6875</v>
       </c>
       <c r="K48">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L48" s="11">
+        <v>4</v>
+      </c>
+      <c r="L48" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M48" s="10">
+      <c r="M48" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N48" s="11">
+      <c r="N48" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>240.00000000000006</v>
-      </c>
-      <c r="O48" s="11">
+        <v>60.000000000000014</v>
+      </c>
+      <c r="O48" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -24718,25 +24717,25 @@
         <f>VLOOKUP(F49,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J49" s="9">
+      <c r="J49" s="8">
         <v>0.70833333333333304</v>
       </c>
       <c r="K49">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L49" s="11">
+        <v>4</v>
+      </c>
+      <c r="L49" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M49" s="10">
+      <c r="M49" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N49" s="11">
+      <c r="N49" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
-      </c>
-      <c r="O49" s="11">
+        <v>105</v>
+      </c>
+      <c r="O49" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -24768,25 +24767,25 @@
         <f>VLOOKUP(F50,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J50" s="9">
+      <c r="J50" s="8">
         <v>0.72916666666666696</v>
       </c>
       <c r="K50">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L50" s="11">
+        <v>1</v>
+      </c>
+      <c r="L50" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M50" s="10">
+      <c r="M50" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N50" s="11">
+      <c r="N50" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>35.199999999999996</v>
-      </c>
-      <c r="O50" s="11">
+        <v>175.99999999999997</v>
+      </c>
+      <c r="O50" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -24818,25 +24817,25 @@
         <f>VLOOKUP(F51,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J51" s="9">
+      <c r="J51" s="8">
         <v>0.75</v>
       </c>
       <c r="K51">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L51" s="11">
+        <v>4</v>
+      </c>
+      <c r="L51" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M51" s="10">
+      <c r="M51" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N51" s="11">
+      <c r="N51" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>120.00000000000003</v>
-      </c>
-      <c r="O51" s="11">
+        <v>60.000000000000014</v>
+      </c>
+      <c r="O51" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -24868,25 +24867,25 @@
         <f>VLOOKUP(F52,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J52" s="9">
+      <c r="J52" s="8">
         <v>0.77083333333333304</v>
       </c>
       <c r="K52">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L52" s="11">
+        <v>4</v>
+      </c>
+      <c r="L52" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M52" s="10">
+      <c r="M52" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N52" s="11">
+      <c r="N52" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="O52" s="11">
+        <v>105</v>
+      </c>
+      <c r="O52" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -24918,25 +24917,25 @@
         <f>VLOOKUP(F53,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J53" s="9">
+      <c r="J53" s="8">
         <v>0.79166666666666696</v>
       </c>
       <c r="K53">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L53" s="11">
+        <v>3</v>
+      </c>
+      <c r="L53" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M53" s="10">
+      <c r="M53" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N53" s="11">
+      <c r="N53" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>87.999999999999986</v>
-      </c>
-      <c r="O53" s="11">
+        <v>58.666666666666657</v>
+      </c>
+      <c r="O53" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -24968,25 +24967,25 @@
         <f>VLOOKUP(F54,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J54" s="9">
+      <c r="J54" s="8">
         <v>0.8125</v>
       </c>
       <c r="K54">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L54" s="11">
+        <v>2</v>
+      </c>
+      <c r="L54" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M54" s="10">
+      <c r="M54" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N54" s="11">
+      <c r="N54" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>60.000000000000014</v>
-      </c>
-      <c r="O54" s="11">
+        <v>120.00000000000003</v>
+      </c>
+      <c r="O54" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -25018,25 +25017,25 @@
         <f>VLOOKUP(F55,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J55" s="9">
+      <c r="J55" s="8">
         <v>0.83333333333333304</v>
       </c>
       <c r="K55">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L55" s="11">
+        <v>4</v>
+      </c>
+      <c r="L55" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M55" s="10">
+      <c r="M55" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N55" s="11">
+      <c r="N55" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="O55" s="11">
+        <v>105</v>
+      </c>
+      <c r="O55" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -25068,25 +25067,25 @@
         <f>VLOOKUP(F56,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J56" s="9">
+      <c r="J56" s="8">
         <v>0.85416666666666696</v>
       </c>
       <c r="K56">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L56" s="11">
+        <v>5</v>
+      </c>
+      <c r="L56" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M56" s="10">
+      <c r="M56" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N56" s="11">
+      <c r="N56" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>87.999999999999986</v>
-      </c>
-      <c r="O56" s="11">
+        <v>35.199999999999996</v>
+      </c>
+      <c r="O56" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -25118,25 +25117,25 @@
         <f>VLOOKUP(F57,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J57" s="9">
+      <c r="J57" s="8">
         <v>0.875</v>
       </c>
       <c r="K57">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L57" s="11">
+        <v>5</v>
+      </c>
+      <c r="L57" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M57" s="10">
+      <c r="M57" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N57" s="11">
+      <c r="N57" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>120.00000000000003</v>
-      </c>
-      <c r="O57" s="11">
+        <v>48.000000000000014</v>
+      </c>
+      <c r="O57" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -25168,25 +25167,25 @@
         <f>VLOOKUP(F58,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J58" s="9">
+      <c r="J58" s="8">
         <v>0.89583333333333304</v>
       </c>
       <c r="K58">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L58" s="11">
+        <v>4</v>
+      </c>
+      <c r="L58" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M58" s="10">
+      <c r="M58" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N58" s="11">
+      <c r="N58" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>420</v>
-      </c>
-      <c r="O58" s="11">
+        <v>105</v>
+      </c>
+      <c r="O58" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -25218,25 +25217,25 @@
         <f>VLOOKUP(F59,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J59" s="9">
+      <c r="J59" s="8">
         <v>0.91666666666666696</v>
       </c>
       <c r="K59">
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="L59" s="11">
+      <c r="L59" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M59" s="10">
+      <c r="M59" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N59" s="11">
+      <c r="N59" s="10">
         <f t="shared" ca="1" si="2"/>
         <v>43.999999999999993</v>
       </c>
-      <c r="O59" s="11">
+      <c r="O59" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -25268,25 +25267,25 @@
         <f>VLOOKUP(F60,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J60" s="9">
+      <c r="J60" s="8">
         <v>0.9375</v>
       </c>
       <c r="K60">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L60" s="11">
+        <v>2</v>
+      </c>
+      <c r="L60" s="10">
         <f t="shared" si="1"/>
         <v>240.00000000000006</v>
       </c>
-      <c r="M60" s="10">
+      <c r="M60" s="9">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N60" s="11">
+      <c r="N60" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>60.000000000000014</v>
-      </c>
-      <c r="O60" s="11">
+        <v>120.00000000000003</v>
+      </c>
+      <c r="O60" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>240.00000000000006</v>
       </c>
@@ -25318,25 +25317,25 @@
         <f>VLOOKUP(F61,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J61" s="9">
+      <c r="J61" s="8">
         <v>0.95833333333333304</v>
       </c>
       <c r="K61">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="L61" s="11">
+      <c r="L61" s="10">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="M61" s="10">
+      <c r="M61" s="9">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="N61" s="11">
+      <c r="N61" s="10">
         <f t="shared" ca="1" si="2"/>
         <v>420</v>
       </c>
-      <c r="O61" s="11">
+      <c r="O61" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>420</v>
       </c>
@@ -25368,25 +25367,25 @@
         <f>VLOOKUP(F62,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="J62" s="9">
+      <c r="J62" s="8">
         <v>0.97916666666666696</v>
       </c>
       <c r="K62">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="L62" s="11">
+      <c r="L62" s="10">
         <f t="shared" si="1"/>
         <v>175.99999999999997</v>
       </c>
-      <c r="M62" s="10">
+      <c r="M62" s="9">
         <v>2.0370370370370369E-3</v>
       </c>
-      <c r="N62" s="11">
+      <c r="N62" s="10">
         <f t="shared" ca="1" si="2"/>
         <v>35.199999999999996</v>
       </c>
-      <c r="O62" s="11">
+      <c r="O62" s="10">
         <f t="shared" ca="1" si="3"/>
         <v>175.99999999999997</v>
       </c>
@@ -25418,13 +25417,13 @@
         <f>VLOOKUP(F63,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="K63" s="11">
+      <c r="K63" s="10">
         <f ca="1">SUM(K15:K62)</f>
-        <v>147</v>
-      </c>
-      <c r="L63" s="11"/>
-      <c r="N63" s="11"/>
-      <c r="O63" s="11">
+        <v>156</v>
+      </c>
+      <c r="L63" s="10"/>
+      <c r="N63" s="10"/>
+      <c r="O63" s="10">
         <f ca="1">AVERAGE(O15:O62)</f>
         <v>278.66666666666669</v>
       </c>
@@ -25456,9 +25455,9 @@
         <f>VLOOKUP(F64,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="O64" s="12">
+      <c r="O64" s="11">
         <f ca="1">(K63/O63)</f>
-        <v>0.52751196172248804</v>
+        <v>0.55980861244019131</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
@@ -25488,9 +25487,9 @@
         <f>VLOOKUP(F65,Vendas!A:C,3,0)</f>
         <v>Eletrônicos</v>
       </c>
-      <c r="O65" s="11">
+      <c r="O65" s="10">
         <f ca="1">SUMPRODUCT(K15:K62,L15:L62)/SUM(K15:K62)</f>
-        <v>274.8299319727891</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>